<commit_message>
hydropower update: improved forecast structure, improved storage start levels, adding pumps to psOpen and psClosed
</commit_message>
<xml_diff>
--- a/src_files/data_files/unitdata_TYNDP-2020.xlsx
+++ b/src_files/data_files/unitdata_TYNDP-2020.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\NEBB-alt\src_files\data_files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BB\bb-master\north_european_model\src_files\data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D259F6AF-E62A-4E62-9D6A-BD92896AA94E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DD2DBD-E474-40BE-901B-B1FA57244E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17880" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="unitdata" sheetId="1" r:id="rId1"/>
+    <sheet name="unitdata_pumps" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">unitdata!$A$1:$H$3825</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">unitdata_pumps!$A$1:$H$15</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14727" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14791" uniqueCount="118">
   <si>
     <t>Generator_ID</t>
   </si>
@@ -384,6 +386,15 @@
   </si>
   <si>
     <t>node_suffix_output2</t>
+  </si>
+  <si>
+    <t>PS Open pump</t>
+  </si>
+  <si>
+    <t>PS Closed pump</t>
+  </si>
+  <si>
+    <t>all</t>
   </si>
 </sst>
 </file>
@@ -784,9 +795,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3825"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2610" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2625" sqref="D2625"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -80037,4 +80048,358 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6D164EB-45DC-4B94-9982-6DD8B5904CD1}">
+  <dimension ref="A1:H15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A16" sqref="A16:XFD92"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1361</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" t="s">
+        <v>117</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4">
+        <v>2424</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1850</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4">
+        <v>84</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4">
+        <v>1030</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4">
+        <v>172</v>
+      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1150</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" s="4">
+        <v>6068</v>
+      </c>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3142</v>
+      </c>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1950</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>900</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="4">
+        <v>1486</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>116</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2744</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H15" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H15">
+      <sortCondition ref="C1:C15"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>